<commit_message>
removed the page config function, made the forgot password and username popups, hid the constraints tab, that should be all
</commit_message>
<xml_diff>
--- a/Version 3.0/sheets/final_timetable.xlsx
+++ b/Version 3.0/sheets/final_timetable.xlsx
@@ -508,7 +508,11 @@
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>CSC442</t>
+        </is>
+      </c>
       <c r="K2" t="inlineStr"/>
     </row>
     <row r="3">
@@ -535,11 +539,7 @@
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>CSC423</t>
-        </is>
-      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
           <t>CSC423</t>
@@ -547,11 +547,7 @@
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>CSC111</t>
-        </is>
-      </c>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
@@ -701,11 +697,7 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
@@ -743,8 +735,16 @@
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>CSC425</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>CSC442</t>
+        </is>
+      </c>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
     </row>
@@ -827,13 +827,13 @@
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>MAT111</t>
+        </is>
+      </c>
       <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>CHM111</t>
-        </is>
-      </c>
+      <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
     </row>
@@ -845,20 +845,24 @@
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>CST111</t>
+        </is>
+      </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
+      <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr">
         <is>
-          <t>CSC424</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr"/>
+          <t>CHM111</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>CHM111</t>
+        </is>
+      </c>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
     </row>
@@ -1120,14 +1124,18 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr">
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
         <is>
           <t>CSC423</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>CSC423</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1170,16 +1178,8 @@
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>BIO111</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>BIO111</t>
-        </is>
-      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
@@ -1333,7 +1333,11 @@
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>CSC111</t>
+        </is>
+      </c>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
@@ -1398,24 +1402,20 @@
           <t>LT 1</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr">
+      <c r="B20" t="inlineStr">
         <is>
           <t>MAT111</t>
         </is>
       </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>MAT111</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>MAT112</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>MAT112</t>
-        </is>
-      </c>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
@@ -1427,29 +1427,21 @@
           <t>LT 2</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
         <is>
           <t>CST111</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>CST111</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>TMC421</t>
-        </is>
-      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>GST111</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>TMC111</t>
-        </is>
-      </c>
+      <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
@@ -1501,8 +1493,16 @@
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>CSC441</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>CSC441</t>
+        </is>
+      </c>
       <c r="K24" t="inlineStr"/>
     </row>
     <row r="25">
@@ -1696,7 +1696,11 @@
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
     </row>
@@ -1711,11 +1715,7 @@
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>CSC425</t>
-        </is>
-      </c>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
@@ -1768,16 +1768,8 @@
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>CSC111</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>CSC111</t>
-        </is>
-      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
@@ -1793,11 +1785,7 @@
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>CSC442</t>
-        </is>
-      </c>
+      <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
     </row>
@@ -1832,16 +1820,8 @@
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>CIS421</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>CIS421</t>
-        </is>
-      </c>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1888,11 +1868,19 @@
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>CIS421</t>
+        </is>
+      </c>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>CSC111</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1903,16 +1891,8 @@
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr"/>
@@ -1927,11 +1907,7 @@
       </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>CSC442</t>
-        </is>
-      </c>
+      <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
@@ -2019,17 +1995,13 @@
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>PHY111</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>PHY111</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>TMC111</t>
+        </is>
+      </c>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
     </row>
@@ -2047,8 +2019,16 @@
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr"/>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>MAT112</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>MAT112</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2094,7 +2074,11 @@
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>CSC425</t>
+        </is>
+      </c>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
@@ -2109,7 +2093,11 @@
       </c>
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr"/>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr"/>
@@ -2356,21 +2344,17 @@
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>CSC425</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>CSC425</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>CSC425</t>
-        </is>
-      </c>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -2434,7 +2418,11 @@
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
@@ -2487,7 +2475,11 @@
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>CIS421</t>
+        </is>
+      </c>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
     </row>
@@ -2537,11 +2529,7 @@
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>BIO111</t>
-        </is>
-      </c>
+      <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
@@ -2603,26 +2591,18 @@
           <t>LT 2</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>EDS421</t>
+        </is>
+      </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>MAT111</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>MAT111</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>CSC441</t>
-        </is>
-      </c>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
     </row>
@@ -2675,7 +2655,11 @@
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
-      <c r="K24" t="inlineStr"/>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>CSC442</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2691,7 +2675,11 @@
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr"/>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
       <c r="K25" t="inlineStr"/>
     </row>
     <row r="26">
@@ -2844,12 +2832,12 @@
           <t>Bio Chem Lab 1</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CSC441</t>
-        </is>
-      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>BIO111</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
@@ -3003,11 +2991,7 @@
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
@@ -3042,11 +3026,7 @@
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>CSC442</t>
-        </is>
-      </c>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
@@ -3080,7 +3060,11 @@
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>CSC111</t>
+        </is>
+      </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
@@ -3112,7 +3096,11 @@
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>BIO111</t>
+        </is>
+      </c>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
@@ -3166,12 +3154,12 @@
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>EDS421</t>
-        </is>
-      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>TMC421</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
@@ -3186,7 +3174,11 @@
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>GST111</t>
+        </is>
+      </c>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
@@ -3235,7 +3227,11 @@
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
-      <c r="C24" t="inlineStr"/>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>

</xml_diff>

<commit_message>
fixed the expected output
</commit_message>
<xml_diff>
--- a/Version 3.0/sheets/final_timetable.xlsx
+++ b/Version 3.0/sheets/final_timetable.xlsx
@@ -508,11 +508,7 @@
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>CSC442</t>
-        </is>
-      </c>
+      <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
     </row>
     <row r="3">
@@ -540,14 +536,14 @@
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>CSC423</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
@@ -662,7 +658,11 @@
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>CSC423</t>
+        </is>
+      </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
@@ -700,7 +700,11 @@
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>CSC425</t>
+        </is>
+      </c>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
@@ -717,7 +721,11 @@
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>CSC111</t>
+        </is>
+      </c>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
@@ -735,16 +743,8 @@
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>CSC425</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>CSC442</t>
-        </is>
-      </c>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
     </row>
@@ -822,17 +822,29 @@
           <t>LT 1</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>DLD221</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>DLD221</t>
+        </is>
+      </c>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr">
         <is>
-          <t>MAT111</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr"/>
+          <t>PHY111</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>PHY111</t>
+        </is>
+      </c>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
@@ -845,25 +857,21 @@
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>CST111</t>
-        </is>
-      </c>
+      <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>CHM111</t>
-        </is>
-      </c>
+      <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr">
         <is>
-          <t>CHM111</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr"/>
+          <t>CIT111</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>CIT111</t>
+        </is>
+      </c>
       <c r="K21" t="inlineStr"/>
     </row>
     <row r="22">
@@ -946,8 +954,16 @@
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr"/>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>CSC441</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>CSC441</t>
+        </is>
+      </c>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr"/>
     </row>
@@ -1126,16 +1142,8 @@
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>CSC423</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>CSC423</t>
-        </is>
-      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1304,7 +1312,11 @@
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
       <c r="K14" t="inlineStr"/>
     </row>
     <row r="15">
@@ -1333,11 +1345,7 @@
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>CSC111</t>
-        </is>
-      </c>
+      <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
@@ -1359,8 +1367,16 @@
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>CSC423</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>CSC423</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1402,21 +1418,17 @@
           <t>LT 1</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>MAT111</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>MAT111</t>
-        </is>
-      </c>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>TMC421</t>
+        </is>
+      </c>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
@@ -1429,16 +1441,8 @@
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>CST111</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>GST111</t>
-        </is>
-      </c>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
@@ -1493,16 +1497,8 @@
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>CSC441</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>CSC441</t>
-        </is>
-      </c>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr"/>
     </row>
     <row r="25">
@@ -1696,11 +1692,7 @@
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
+      <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
     </row>
@@ -1763,8 +1755,16 @@
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>CSC442</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>CSC442</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
@@ -1816,7 +1816,11 @@
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>BIO111</t>
+        </is>
+      </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
@@ -1868,19 +1872,11 @@
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>CIS421</t>
-        </is>
-      </c>
+      <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>CSC111</t>
-        </is>
-      </c>
+      <c r="K13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1922,8 +1918,16 @@
           <t>Hall 204</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
@@ -1977,8 +1981,16 @@
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>CIS421</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>CIS421</t>
+        </is>
+      </c>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
@@ -1993,16 +2005,28 @@
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>MAT112</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>MAT112</t>
+        </is>
+      </c>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr">
         <is>
-          <t>TMC111</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr"/>
+          <t>CST111</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>CST111</t>
+        </is>
+      </c>
       <c r="K20" t="inlineStr"/>
     </row>
     <row r="21">
@@ -2016,19 +2040,19 @@
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>MAT111</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>MAT111</t>
+        </is>
+      </c>
       <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>MAT112</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>MAT112</t>
-        </is>
-      </c>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2074,11 +2098,7 @@
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>CSC425</t>
-        </is>
-      </c>
+      <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
@@ -2093,17 +2113,21 @@
       </c>
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
+      <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr"/>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
       <c r="K25" t="inlineStr"/>
     </row>
     <row r="26">
@@ -2344,16 +2368,20 @@
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>CSC425</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>CSC111</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>CSC111</t>
+        </is>
+      </c>
       <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
@@ -2418,11 +2446,7 @@
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
+      <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
@@ -2475,11 +2499,7 @@
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>CIS421</t>
-        </is>
-      </c>
+      <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
     </row>
@@ -2510,8 +2530,16 @@
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>CSC425</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>CSC425</t>
+        </is>
+      </c>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
@@ -2528,7 +2556,11 @@
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>CSC442</t>
+        </is>
+      </c>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
@@ -2591,15 +2623,15 @@
           <t>LT 2</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>EDS421</t>
-        </is>
-      </c>
+      <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>CHM111</t>
+        </is>
+      </c>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr"/>
@@ -2655,11 +2687,7 @@
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>CSC442</t>
-        </is>
-      </c>
+      <c r="K24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2675,11 +2703,7 @@
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
+      <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
     </row>
     <row r="26">
@@ -2832,11 +2856,7 @@
           <t>Bio Chem Lab 1</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>BIO111</t>
-        </is>
-      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
@@ -3060,11 +3080,7 @@
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>CSC111</t>
-        </is>
-      </c>
+      <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
@@ -3096,11 +3112,7 @@
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>BIO111</t>
-        </is>
-      </c>
+      <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
@@ -3151,12 +3163,16 @@
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>MAT111</t>
+        </is>
+      </c>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>TMC421</t>
+          <t>TMC111</t>
         </is>
       </c>
       <c r="G20" t="inlineStr"/>
@@ -3174,11 +3190,7 @@
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>GST111</t>
-        </is>
-      </c>
+      <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
@@ -3227,11 +3239,7 @@
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
+      <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>

</xml_diff>

<commit_message>
Connected the create timetable button to the script
</commit_message>
<xml_diff>
--- a/Version 3.0/sheets/final_timetable.xlsx
+++ b/Version 3.0/sheets/final_timetable.xlsx
@@ -537,13 +537,13 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>CSC423</t>
+        </is>
+      </c>
       <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
@@ -658,11 +658,7 @@
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>CSC423</t>
-        </is>
-      </c>
+      <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
@@ -700,14 +696,18 @@
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>CSC425</t>
-        </is>
-      </c>
+      <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>CSC442</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>CSC442</t>
+        </is>
+      </c>
       <c r="K13" t="inlineStr"/>
     </row>
     <row r="14">
@@ -721,11 +721,7 @@
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>CSC111</t>
-        </is>
-      </c>
+      <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
@@ -824,27 +820,19 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>DLD221</t>
+          <t>GST111</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>DLD221</t>
+          <t>GST111</t>
         </is>
       </c>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>PHY111</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>PHY111</t>
-        </is>
-      </c>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
@@ -862,17 +850,17 @@
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>CIT111</t>
-        </is>
-      </c>
+      <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr">
         <is>
-          <t>CIT111</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr"/>
+          <t>MAT112</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>MAT112</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -954,16 +942,8 @@
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>CSC441</t>
-        </is>
-      </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>CSC441</t>
-        </is>
-      </c>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr"/>
     </row>
@@ -1237,8 +1217,16 @@
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>BIO111</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>BIO111</t>
+        </is>
+      </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
@@ -1312,11 +1300,7 @@
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
+      <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
     </row>
     <row r="15">
@@ -1333,7 +1317,11 @@
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>CSC425</t>
+        </is>
+      </c>
       <c r="K15" t="inlineStr"/>
     </row>
     <row r="16">
@@ -1424,13 +1412,17 @@
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>TMC421</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>MAT111</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>MAT111</t>
+        </is>
+      </c>
       <c r="K20" t="inlineStr"/>
     </row>
     <row r="21">
@@ -1447,7 +1439,11 @@
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
       <c r="K21" t="inlineStr"/>
     </row>
     <row r="22">
@@ -1515,8 +1511,16 @@
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr"/>
-      <c r="K25" t="inlineStr"/>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>CIS421</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>CIS421</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1709,8 +1713,16 @@
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
       <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
@@ -1755,16 +1767,8 @@
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>CSC442</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>CSC442</t>
-        </is>
-      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
@@ -1816,11 +1820,7 @@
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>BIO111</t>
-        </is>
-      </c>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
@@ -1918,16 +1918,8 @@
           <t>Hall 204</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
@@ -1981,16 +1973,8 @@
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>CIS421</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>CIS421</t>
-        </is>
-      </c>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
@@ -2004,29 +1988,21 @@
       </c>
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>CIT111</t>
+        </is>
+      </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>MAT112</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>MAT112</t>
-        </is>
-      </c>
+          <t>CIT111</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>CST111</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>CST111</t>
-        </is>
-      </c>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
     </row>
     <row r="21">
@@ -2038,18 +2014,14 @@
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>MAT111</t>
+        </is>
+      </c>
       <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>MAT111</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>MAT111</t>
-        </is>
-      </c>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
@@ -2116,18 +2088,18 @@
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>CSC111</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>CSC111</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
     </row>
     <row r="26">
@@ -2367,21 +2339,21 @@
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>CSC441</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>CSC441</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>CSC111</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>CSC111</t>
-        </is>
-      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
@@ -2449,8 +2421,16 @@
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2530,16 +2510,8 @@
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>CSC425</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>CSC425</t>
-        </is>
-      </c>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
@@ -2556,11 +2528,7 @@
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>CSC442</t>
-        </is>
-      </c>
+      <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
@@ -2610,11 +2578,23 @@
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>CSC442</t>
+        </is>
+      </c>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>CHM111</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>CHM111</t>
+        </is>
+      </c>
       <c r="K20" t="inlineStr"/>
     </row>
     <row r="21">
@@ -2627,15 +2607,15 @@
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>CHM111</t>
-        </is>
-      </c>
+      <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>EDS421</t>
+        </is>
+      </c>
       <c r="K21" t="inlineStr"/>
     </row>
     <row r="22">
@@ -3163,18 +3143,14 @@
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>MAT111</t>
-        </is>
-      </c>
+      <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>TMC111</t>
         </is>
       </c>
+      <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr"/>
@@ -3188,7 +3164,11 @@
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>TMC421</t>
+        </is>
+      </c>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>

</xml_diff>

<commit_message>
Tried to place courses by heirachy. But it just messed up the solution.
</commit_message>
<xml_diff>
--- a/Version 3.0/sheets/final_timetable.xlsx
+++ b/Version 3.0/sheets/final_timetable.xlsx
@@ -535,13 +535,17 @@
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>CSC423</t>
-        </is>
-      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>CSC442</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>CSC442</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
@@ -698,16 +702,8 @@
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>CSC442</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>CSC442</t>
-        </is>
-      </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
     </row>
     <row r="14">
@@ -793,7 +789,11 @@
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>CSC423</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -818,19 +818,19 @@
           <t>LT 1</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>GST111</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>GST111</t>
-        </is>
-      </c>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>MAT112</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>MAT112</t>
+        </is>
+      </c>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr"/>
@@ -849,18 +849,22 @@
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>CSC425</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>CIT111</t>
+        </is>
+      </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>MAT112</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>MAT112</t>
-        </is>
-      </c>
+          <t>CIT111</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1217,16 +1221,8 @@
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>BIO111</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>BIO111</t>
-        </is>
-      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
@@ -1312,14 +1308,22 @@
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>CSC425</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>CSC425</t>
+        </is>
+      </c>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr">
         <is>
-          <t>CSC425</t>
+          <t>BIO111</t>
         </is>
       </c>
       <c r="K15" t="inlineStr"/>
@@ -1353,18 +1357,14 @@
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
       <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>CSC423</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>CSC423</t>
-        </is>
-      </c>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1413,17 +1413,13 @@
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>MAT111</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>MAT111</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1439,11 +1435,7 @@
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
+      <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
     </row>
     <row r="22">
@@ -1511,16 +1503,8 @@
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>CIS421</t>
-        </is>
-      </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>CIS421</t>
-        </is>
-      </c>
+      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1677,8 +1661,16 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>CIS421</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>CIS421</t>
+        </is>
+      </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
@@ -1713,16 +1705,8 @@
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
@@ -1788,8 +1772,16 @@
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>BIO111</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>BIO111</t>
+        </is>
+      </c>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
     </row>
@@ -1840,8 +1832,16 @@
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>CSC441</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>CSC441</t>
+        </is>
+      </c>
       <c r="K11" t="inlineStr"/>
     </row>
     <row r="12">
@@ -1873,8 +1873,16 @@
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>CSC423</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>CSC423</t>
+        </is>
+      </c>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
     </row>
@@ -1988,22 +1996,30 @@
       </c>
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>CIT111</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>CIT111</t>
-        </is>
-      </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr"/>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>DLD221</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>DLD221</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2013,12 +2029,12 @@
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>MAT111</t>
-        </is>
-      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>TMC111</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
@@ -2088,16 +2104,8 @@
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>CSC111</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>CSC111</t>
-        </is>
-      </c>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
@@ -2290,7 +2298,11 @@
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>CSC111</t>
+        </is>
+      </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
@@ -2339,16 +2351,8 @@
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>CSC441</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>CSC441</t>
-        </is>
-      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
@@ -2421,16 +2425,8 @@
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2528,8 +2524,16 @@
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
@@ -2549,7 +2553,11 @@
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>CSC442</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2578,24 +2586,20 @@
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>CSC442</t>
-        </is>
-      </c>
+      <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr">
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr">
         <is>
           <t>CHM111</t>
         </is>
       </c>
-      <c r="J20" t="inlineStr">
+      <c r="K20" t="inlineStr">
         <is>
           <t>CHM111</t>
         </is>
       </c>
-      <c r="K20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2607,15 +2611,19 @@
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>MAT111</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>MAT111</t>
+        </is>
+      </c>
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>EDS421</t>
-        </is>
-      </c>
+      <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
     </row>
     <row r="22">
@@ -3145,11 +3153,7 @@
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>TMC111</t>
-        </is>
-      </c>
+      <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
@@ -3164,11 +3168,7 @@
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>TMC421</t>
-        </is>
-      </c>
+      <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>

</xml_diff>

<commit_message>
Renamed the frontend folder
</commit_message>
<xml_diff>
--- a/Version 3.0/sheets/final_timetable.xlsx
+++ b/Version 3.0/sheets/final_timetable.xlsx
@@ -517,7 +517,11 @@
           <t>Bio Chem Lab 2</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>CSC423</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
@@ -541,11 +545,7 @@
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>CSC423</t>
-        </is>
-      </c>
+      <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
     </row>
@@ -593,16 +593,8 @@
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>CSC111</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>CSC111</t>
-        </is>
-      </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
@@ -701,8 +693,16 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
@@ -724,7 +724,11 @@
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
       <c r="K14" t="inlineStr"/>
     </row>
     <row r="15">
@@ -741,11 +745,7 @@
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>BIO111</t>
-        </is>
-      </c>
+      <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
     </row>
     <row r="16">
@@ -773,14 +773,14 @@
       </c>
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
+      <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>BIO111</t>
+        </is>
+      </c>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
@@ -815,16 +815,8 @@
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr"/>
     </row>
@@ -837,16 +829,8 @@
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>MAT111</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>MAT111</t>
-        </is>
-      </c>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr"/>
@@ -863,14 +847,10 @@
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>GST111</t>
-        </is>
-      </c>
+      <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">
         <is>
-          <t>GST111</t>
+          <t>MAT111</t>
         </is>
       </c>
       <c r="H21" t="inlineStr"/>
@@ -1181,8 +1161,16 @@
           <t>Chem Prac. Lab</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>CSC425</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>CSC425</t>
+        </is>
+      </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
@@ -1301,8 +1289,16 @@
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>CSC442</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>CSC442</t>
+        </is>
+      </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
@@ -1406,16 +1402,16 @@
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>EDS421</t>
+        </is>
+      </c>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>MAT111</t>
-        </is>
-      </c>
+      <c r="K20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1424,30 +1420,22 @@
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>MAT112</t>
+        </is>
+      </c>
       <c r="D21" t="inlineStr">
         <is>
           <t>MAT112</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>MAT112</t>
-        </is>
-      </c>
+      <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>CST111</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>CST111</t>
-        </is>
-      </c>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
     </row>
     <row r="22">
@@ -1760,11 +1748,7 @@
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>CSC425</t>
-        </is>
-      </c>
+      <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
     </row>
@@ -1878,16 +1862,8 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>BIO111</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>BIO111</t>
-        </is>
-      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
@@ -1905,7 +1881,11 @@
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
@@ -1942,8 +1922,16 @@
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>CIS421</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>CIS421</t>
+        </is>
+      </c>
       <c r="K17" t="inlineStr"/>
     </row>
     <row r="18">
@@ -1988,25 +1976,25 @@
       </c>
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>CIT111</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>CIT111</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>MAT111</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>MAT111</t>
+        </is>
+      </c>
       <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>EDS421</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>TMC421</t>
+        </is>
+      </c>
       <c r="K20" t="inlineStr"/>
     </row>
     <row r="21">
@@ -2036,8 +2024,16 @@
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>CSC441</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>CSC441</t>
+        </is>
+      </c>
       <c r="H22" t="inlineStr"/>
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
@@ -2089,8 +2085,16 @@
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr"/>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>CSC111</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>CSC111</t>
+        </is>
+      </c>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
     </row>
@@ -2249,16 +2253,8 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>CSC425</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>CSC425</t>
-        </is>
-      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
@@ -2290,11 +2286,7 @@
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>CSC111</t>
-        </is>
-      </c>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
@@ -2446,11 +2438,7 @@
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
@@ -2517,21 +2505,9 @@
       </c>
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>CSC442</t>
-        </is>
-      </c>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
@@ -2565,8 +2541,16 @@
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
@@ -2584,8 +2568,16 @@
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>CST111</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>CST111</t>
+        </is>
+      </c>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
     </row>
@@ -2600,7 +2592,11 @@
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>CSC111</t>
+        </is>
+      </c>
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
@@ -2649,16 +2645,8 @@
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>CSC423</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>CSC423</t>
-        </is>
-      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
@@ -2921,16 +2909,8 @@
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>CIS421</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>CIS421</t>
-        </is>
-      </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
@@ -2979,8 +2959,16 @@
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>CSC423</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>CSC423</t>
+        </is>
+      </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
@@ -3029,7 +3017,11 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>CSC442</t>
+        </is>
+      </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
@@ -3147,7 +3139,11 @@
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>TMC111</t>
+        </is>
+      </c>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
@@ -3165,8 +3161,16 @@
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>CHM111</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>CHM111</t>
+        </is>
+      </c>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
@@ -3283,16 +3287,8 @@
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>CSC441</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>CSC441</t>
-        </is>
-      </c>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>

</xml_diff>

<commit_message>
Worked on the student booking constraint and set up the emailing system.
</commit_message>
<xml_diff>
--- a/Version 3.0/sheets/final_timetable.xlsx
+++ b/Version 3.0/sheets/final_timetable.xlsx
@@ -517,11 +517,7 @@
           <t>Bio Chem Lab 2</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>CSC423</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
@@ -645,8 +641,16 @@
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
@@ -693,16 +697,8 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
@@ -724,11 +720,7 @@
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
+      <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
     </row>
     <row r="15">
@@ -745,8 +737,16 @@
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>CSC423</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>CSC423</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -776,11 +776,7 @@
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>BIO111</t>
-        </is>
-      </c>
+      <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
@@ -829,7 +825,11 @@
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>MAT111</t>
+        </is>
+      </c>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
@@ -847,14 +847,22 @@
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>MAT111</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>EDS421</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>TMC421</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>TMC111</t>
+        </is>
+      </c>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
     </row>
@@ -923,7 +931,11 @@
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr"/>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>BIO111</t>
+        </is>
+      </c>
       <c r="K25" t="inlineStr"/>
     </row>
     <row r="26">
@@ -1161,16 +1173,8 @@
           <t>Chem Prac. Lab</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>CSC425</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>CSC425</t>
-        </is>
-      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
@@ -1194,8 +1198,16 @@
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>CSC425</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>CSC425</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1276,7 +1288,11 @@
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
@@ -1289,16 +1305,8 @@
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>CSC442</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>CSC442</t>
-        </is>
-      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
@@ -1337,7 +1345,11 @@
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>CSC442</t>
+        </is>
+      </c>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
     </row>
@@ -1350,8 +1362,16 @@
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>CIS421</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>CIS421</t>
+        </is>
+      </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
@@ -1402,11 +1422,7 @@
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>EDS421</t>
-        </is>
-      </c>
+      <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr"/>
@@ -1420,20 +1436,20 @@
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>MAT112</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>MAT112</t>
-        </is>
-      </c>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>CIT111</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>CIT111</t>
+        </is>
+      </c>
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
@@ -1761,7 +1777,11 @@
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
@@ -1795,7 +1815,11 @@
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>CSC425</t>
+        </is>
+      </c>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
@@ -1881,11 +1905,7 @@
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
+      <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
@@ -1902,8 +1922,16 @@
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>BIO111</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>BIO111</t>
+        </is>
+      </c>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
@@ -1922,16 +1950,8 @@
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>CIS421</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>CIS421</t>
-        </is>
-      </c>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
     </row>
     <row r="18">
@@ -1975,26 +1995,38 @@
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>MAT111</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>MAT111</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>CSC111</t>
+        </is>
+      </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>MAT111</t>
+          <t>CSC111</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>MAT111</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr"/>
+          <t>DLD221</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>DLD221</t>
+        </is>
+      </c>
       <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>TMC421</t>
-        </is>
-      </c>
+      <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
     </row>
     <row r="21">
@@ -2011,8 +2043,16 @@
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr"/>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>MAT112</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>MAT112</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2024,16 +2064,8 @@
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>CSC441</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>CSC441</t>
-        </is>
-      </c>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr"/>
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
@@ -2085,16 +2117,8 @@
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>CSC111</t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>CSC111</t>
-        </is>
-      </c>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
     </row>
@@ -2141,8 +2165,16 @@
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>CSC441</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>CSC441</t>
+        </is>
+      </c>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr"/>
       <c r="I28" t="inlineStr"/>
@@ -2541,16 +2573,8 @@
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
@@ -2568,17 +2592,17 @@
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>CST111</t>
-        </is>
-      </c>
+      <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr">
         <is>
-          <t>CST111</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr"/>
+          <t>CHM111</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>CHM111</t>
+        </is>
+      </c>
       <c r="K20" t="inlineStr"/>
     </row>
     <row r="21">
@@ -2592,11 +2616,7 @@
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>CSC111</t>
-        </is>
-      </c>
+      <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
@@ -2856,7 +2876,11 @@
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>CSC111</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
@@ -2961,12 +2985,12 @@
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
-          <t>CSC423</t>
+          <t>CSC442</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>CSC423</t>
+          <t>CSC442</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
@@ -3017,11 +3041,7 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>CSC442</t>
-        </is>
-      </c>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
@@ -3073,7 +3093,11 @@
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>CSC423</t>
+        </is>
+      </c>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
@@ -3139,11 +3163,7 @@
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>TMC111</t>
-        </is>
-      </c>
+      <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
@@ -3161,16 +3181,8 @@
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>CHM111</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>CHM111</t>
-        </is>
-      </c>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>

</xml_diff>

<commit_message>
changed the population size to 20
</commit_message>
<xml_diff>
--- a/Version 3.0/sheets/final_timetable.xlsx
+++ b/Version 3.0/sheets/final_timetable.xlsx
@@ -505,10 +505,22 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>EDS121</t>
+        </is>
+      </c>
       <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>PHY121</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>PHY121</t>
+        </is>
+      </c>
       <c r="K2" t="inlineStr"/>
     </row>
     <row r="3">
@@ -524,8 +536,16 @@
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>CSC425</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>CSC425</t>
+        </is>
+      </c>
       <c r="K3" t="inlineStr"/>
     </row>
     <row r="4">
@@ -572,7 +592,11 @@
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>CSC225</t>
+        </is>
+      </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
@@ -586,8 +610,16 @@
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>MAT121</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>MAT121</t>
+        </is>
+      </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
@@ -639,18 +671,18 @@
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>MAT122</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>MAT122</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
@@ -737,16 +769,8 @@
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>CSC423</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>CSC423</t>
-        </is>
-      </c>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -789,8 +813,16 @@
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>PHY122</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>PHY122</t>
+        </is>
+      </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
@@ -814,7 +846,11 @@
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr"/>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>MAT225</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -825,11 +861,7 @@
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>MAT111</t>
-        </is>
-      </c>
+      <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
@@ -846,23 +878,15 @@
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>EDS421</t>
-        </is>
-      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>TMC421</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>TMC421</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>TMC111</t>
-        </is>
-      </c>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
     </row>
@@ -931,11 +955,7 @@
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>BIO111</t>
-        </is>
-      </c>
+      <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
     </row>
     <row r="26">
@@ -967,7 +987,11 @@
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr"/>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>EDS421</t>
+        </is>
+      </c>
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
@@ -1089,8 +1113,16 @@
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>CIT224</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>CIT224</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
@@ -1107,7 +1139,11 @@
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>CSC221</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
@@ -1164,8 +1200,16 @@
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>CSC443</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>CSC443</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1198,16 +1242,8 @@
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>CSC425</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>CSC425</t>
-        </is>
-      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1288,11 +1324,7 @@
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
+      <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
@@ -1322,8 +1354,16 @@
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>CSC446</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>CSC446</t>
+        </is>
+      </c>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
@@ -1345,11 +1385,7 @@
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>CSC442</t>
-        </is>
-      </c>
+      <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
     </row>
@@ -1362,21 +1398,21 @@
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>CIS421</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>CIS421</t>
-        </is>
-      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>CSC444</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>CSC444</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1386,7 +1422,11 @@
       </c>
       <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>MAT121</t>
+        </is>
+      </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
@@ -1409,8 +1449,16 @@
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr"/>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>CIT221</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>CIT221</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1440,19 +1488,19 @@
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>CIT111</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>CIT111</t>
-        </is>
-      </c>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr"/>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>CSC223</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>CSC223</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1499,8 +1547,16 @@
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>CSC227</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>CSC227</t>
+        </is>
+      </c>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr"/>
@@ -1713,7 +1769,11 @@
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>CSC425</t>
+        </is>
+      </c>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
     </row>
@@ -1777,11 +1837,7 @@
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
@@ -1815,11 +1871,7 @@
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>CSC425</t>
-        </is>
-      </c>
+      <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
@@ -1871,8 +1923,16 @@
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>CIT141</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>CIT141</t>
+        </is>
+      </c>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
@@ -1892,8 +1952,16 @@
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>MAT226</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>MAT226</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1922,16 +1990,8 @@
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>BIO111</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>BIO111</t>
-        </is>
-      </c>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
@@ -1995,36 +2055,12 @@
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>MAT111</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>MAT111</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>CSC111</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>CSC111</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>DLD221</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>DLD221</t>
-        </is>
-      </c>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
@@ -2043,16 +2079,8 @@
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>MAT112</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>MAT112</t>
-        </is>
-      </c>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2114,7 +2142,11 @@
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr"/>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>TMC121</t>
+        </is>
+      </c>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
@@ -2128,8 +2160,16 @@
           <t>Studio 1</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr"/>
-      <c r="C26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>CSC221</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>CSC221</t>
+        </is>
+      </c>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
@@ -2164,17 +2204,13 @@
       </c>
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>CSC441</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>CSC441</t>
-        </is>
-      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>PHY129</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr"/>
       <c r="I28" t="inlineStr"/>
@@ -2320,8 +2356,16 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>CST121</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>CST121</t>
+        </is>
+      </c>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
     </row>
@@ -2369,7 +2413,11 @@
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>MIS221</t>
+        </is>
+      </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
@@ -2387,8 +2435,16 @@
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>CSC442</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>CSC442</t>
+        </is>
+      </c>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
@@ -2492,7 +2548,11 @@
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>MAT226</t>
+        </is>
+      </c>
       <c r="K14" t="inlineStr"/>
     </row>
     <row r="15">
@@ -2523,8 +2583,16 @@
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>CIT121</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>CIT121</t>
+        </is>
+      </c>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
@@ -2572,8 +2640,16 @@
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>CSC224</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>CSC224</t>
+        </is>
+      </c>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr"/>
@@ -2589,20 +2665,16 @@
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>CSC223</t>
+        </is>
+      </c>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>CHM111</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>CHM111</t>
-        </is>
-      </c>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
     </row>
     <row r="21">
@@ -2653,8 +2725,16 @@
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
-      <c r="K23" t="inlineStr"/>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>MAT229</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>MAT229</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2701,8 +2781,16 @@
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>CSC423</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>CSC423</t>
+        </is>
+      </c>
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr"/>
@@ -2718,8 +2806,16 @@
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr"/>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>GST122</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>GST122</t>
+        </is>
+      </c>
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
@@ -2734,7 +2830,11 @@
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>TMC221</t>
+        </is>
+      </c>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr"/>
       <c r="I28" t="inlineStr"/>
@@ -2753,7 +2853,11 @@
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr"/>
-      <c r="H29" t="inlineStr"/>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>PHY121</t>
+        </is>
+      </c>
       <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr"/>
@@ -2842,8 +2946,16 @@
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>CSC226</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>CSC226</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
@@ -2876,11 +2988,7 @@
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>CSC111</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
@@ -2933,8 +3041,16 @@
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>CSC125</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>CSC125</t>
+        </is>
+      </c>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
@@ -2983,16 +3099,8 @@
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>CSC442</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>CSC442</t>
-        </is>
-      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
@@ -3093,11 +3201,7 @@
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>CSC423</t>
-        </is>
-      </c>
+      <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
@@ -3149,8 +3253,16 @@
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>CSC441</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>CSC441</t>
+        </is>
+      </c>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
@@ -3166,8 +3278,16 @@
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>CSC121</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>CSC121</t>
+        </is>
+      </c>
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
@@ -3264,7 +3384,11 @@
           <t>Studio 1</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>CSC423</t>
+        </is>
+      </c>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
@@ -3301,8 +3425,16 @@
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>MAT225</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>MAT225</t>
+        </is>
+      </c>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr"/>
       <c r="I28" t="inlineStr"/>

</xml_diff>

<commit_message>
can't reach into the constraints file to get the variables. but the saving of session state works.
</commit_message>
<xml_diff>
--- a/Version 3.0/sheets/final_timetable.xlsx
+++ b/Version 3.0/sheets/final_timetable.xlsx
@@ -505,23 +505,19 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>EDS121</t>
-        </is>
-      </c>
+      <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>PHY121</t>
-        </is>
-      </c>
+      <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
         <is>
-          <t>PHY121</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr"/>
+          <t>CSC441</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>CSC441</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -536,16 +532,8 @@
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>CSC425</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>CSC425</t>
-        </is>
-      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
     </row>
     <row r="4">
@@ -592,11 +580,7 @@
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>CSC225</t>
-        </is>
-      </c>
+      <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
@@ -610,17 +594,13 @@
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>MAT121</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>MAT121</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
@@ -671,16 +651,8 @@
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>MAT122</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>MAT122</t>
-        </is>
-      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
@@ -699,8 +671,16 @@
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>MAT229</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>MAT229</t>
+        </is>
+      </c>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
     </row>
@@ -731,7 +711,11 @@
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>CSC425</t>
+        </is>
+      </c>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
@@ -813,16 +797,8 @@
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>PHY122</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>PHY122</t>
-        </is>
-      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
@@ -846,11 +822,7 @@
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>MAT225</t>
-        </is>
-      </c>
+      <c r="K19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -878,11 +850,7 @@
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>TMC421</t>
-        </is>
-      </c>
+      <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
@@ -938,8 +906,16 @@
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
-      <c r="K24" t="inlineStr"/>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>CSC446</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>CSC446</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -955,8 +931,16 @@
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr"/>
-      <c r="K25" t="inlineStr"/>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>GST221</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>GST221</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -983,15 +967,15 @@
       </c>
       <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>MAT225</t>
+        </is>
+      </c>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>EDS421</t>
-        </is>
-      </c>
+      <c r="H27" t="inlineStr"/>
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
@@ -1113,16 +1097,8 @@
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CIT224</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>CIT224</t>
-        </is>
-      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
@@ -1137,13 +1113,17 @@
           <t>Bio Chem Lab 2</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>CSC221</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>CIT121</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>CIT121</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
@@ -1200,16 +1180,8 @@
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>CSC443</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>CSC443</t>
-        </is>
-      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1343,8 +1315,16 @@
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>GST122</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>GST122</t>
+        </is>
+      </c>
       <c r="K14" t="inlineStr"/>
     </row>
     <row r="15">
@@ -1354,23 +1334,23 @@
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>CSC446</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>CSC446</t>
-        </is>
-      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>CIT224</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>CIT224</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1403,16 +1383,8 @@
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>CSC444</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>CSC444</t>
-        </is>
-      </c>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1422,18 +1394,22 @@
       </c>
       <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>MAT121</t>
-        </is>
-      </c>
+      <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>GST121</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>GST121</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1449,16 +1425,8 @@
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>CIT221</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>CIT221</t>
-        </is>
-      </c>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1469,7 +1437,11 @@
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>TMC121</t>
+        </is>
+      </c>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
@@ -1490,17 +1462,13 @@
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr">
+      <c r="I21" t="inlineStr">
         <is>
           <t>CSC223</t>
         </is>
       </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>CSC223</t>
-        </is>
-      </c>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1544,19 +1512,19 @@
       </c>
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>CSC121</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>CSC121</t>
+        </is>
+      </c>
       <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>CSC227</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>CSC227</t>
-        </is>
-      </c>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr"/>
@@ -1570,8 +1538,16 @@
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr"/>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>CSC224</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>CSC224</t>
+        </is>
+      </c>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr"/>
@@ -1590,8 +1566,16 @@
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr"/>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>CSC226</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>CSC226</t>
+        </is>
+      </c>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr"/>
     </row>
@@ -1639,7 +1623,11 @@
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr"/>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>PHY129</t>
+        </is>
+      </c>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr"/>
@@ -1745,7 +1733,11 @@
           <t>Bio Chem Lab 2</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>CSC221</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
@@ -1769,11 +1761,7 @@
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>CSC425</t>
-        </is>
-      </c>
+      <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
     </row>
@@ -1825,8 +1813,16 @@
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>CSC227</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>CSC227</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1838,8 +1834,16 @@
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>CST121</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>CST121</t>
+        </is>
+      </c>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
@@ -1891,7 +1895,11 @@
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>MAT121</t>
+        </is>
+      </c>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
@@ -1920,19 +1928,15 @@
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>CSC225</t>
+        </is>
+      </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>CIT141</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>CIT141</t>
-        </is>
-      </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
@@ -1952,16 +1956,8 @@
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>MAT226</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>MAT226</t>
-        </is>
-      </c>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1970,7 +1966,11 @@
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>CSC423</t>
+        </is>
+      </c>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
@@ -2026,8 +2026,16 @@
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>CIT221</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>CIT221</t>
+        </is>
+      </c>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
     </row>
@@ -2072,7 +2080,11 @@
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>MAT226</t>
+        </is>
+      </c>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
@@ -2106,8 +2118,16 @@
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>MAT122</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>MAT122</t>
+        </is>
+      </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr"/>
@@ -2142,16 +2162,20 @@
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>TMC121</t>
-        </is>
-      </c>
+      <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr"/>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>CSC223</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>CSC223</t>
+        </is>
+      </c>
       <c r="K25" t="inlineStr"/>
     </row>
     <row r="26">
@@ -2160,24 +2184,28 @@
           <t>Studio 1</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>CSC221</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>CSC221</t>
-        </is>
-      </c>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>EDS121</t>
+        </is>
+      </c>
       <c r="I26" t="inlineStr"/>
-      <c r="J26" t="inlineStr"/>
-      <c r="K26" t="inlineStr"/>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>DLD221</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>DLD221</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2204,11 +2232,7 @@
       </c>
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>PHY129</t>
-        </is>
-      </c>
+      <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
@@ -2227,8 +2251,16 @@
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>CIS421</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>CIS421</t>
+        </is>
+      </c>
       <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr"/>
@@ -2323,8 +2355,16 @@
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
       <c r="K2" t="inlineStr"/>
     </row>
     <row r="3">
@@ -2356,16 +2396,8 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>CST121</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>CST121</t>
-        </is>
-      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
     </row>
@@ -2394,8 +2426,16 @@
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>CIT141</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>CIT141</t>
+        </is>
+      </c>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
@@ -2413,12 +2453,12 @@
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>MIS221</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>EDS421</t>
+        </is>
+      </c>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
@@ -2435,14 +2475,10 @@
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>CSC442</t>
-        </is>
-      </c>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
-          <t>CSC442</t>
+          <t>PHY121</t>
         </is>
       </c>
       <c r="I8" t="inlineStr"/>
@@ -2548,11 +2584,7 @@
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>MAT226</t>
-        </is>
-      </c>
+      <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
     </row>
     <row r="15">
@@ -2567,7 +2599,11 @@
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>TMC421</t>
+        </is>
+      </c>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
@@ -2583,16 +2619,8 @@
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>CIT121</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>CIT121</t>
-        </is>
-      </c>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
@@ -2640,18 +2668,18 @@
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>CSC224</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>CSC224</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>CSC221</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>CSC221</t>
+        </is>
+      </c>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr"/>
@@ -2663,13 +2691,17 @@
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>CSC223</t>
-        </is>
-      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>DLD121</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>DLD121</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
@@ -2725,16 +2757,8 @@
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>MAT229</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>MAT229</t>
-        </is>
-      </c>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2748,8 +2772,16 @@
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr"/>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>CSC125</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>CSC125</t>
+        </is>
+      </c>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr"/>
     </row>
@@ -2781,16 +2813,8 @@
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>CSC423</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>CSC423</t>
-        </is>
-      </c>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr"/>
@@ -2806,18 +2830,18 @@
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>GST122</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>GST122</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr"/>
-      <c r="J27" t="inlineStr"/>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>CSC425</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>CSC425</t>
+        </is>
+      </c>
       <c r="K27" t="inlineStr"/>
     </row>
     <row r="28">
@@ -2830,11 +2854,7 @@
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>TMC221</t>
-        </is>
-      </c>
+      <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr"/>
       <c r="I28" t="inlineStr"/>
@@ -2853,11 +2873,7 @@
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr"/>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>PHY121</t>
-        </is>
-      </c>
+      <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr"/>
@@ -2946,16 +2962,8 @@
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>CSC226</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>CSC226</t>
-        </is>
-      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
@@ -3041,16 +3049,8 @@
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>CSC125</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>CSC125</t>
-        </is>
-      </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
@@ -3134,8 +3134,16 @@
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>MAT226</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>MAT226</t>
+        </is>
+      </c>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
@@ -3185,8 +3193,16 @@
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>PHY122</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>PHY122</t>
+        </is>
+      </c>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
@@ -3232,8 +3248,16 @@
           <t>Hall 307</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>CSC444</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>CSC444</t>
+        </is>
+      </c>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
@@ -3253,16 +3277,8 @@
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>CSC441</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>CSC441</t>
-        </is>
-      </c>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
@@ -3280,12 +3296,12 @@
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>CSC121</t>
+          <t>MAT225</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>CSC121</t>
+          <t>MAT225</t>
         </is>
       </c>
       <c r="H20" t="inlineStr"/>
@@ -3354,8 +3370,16 @@
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>MAT121</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>MAT121</t>
+        </is>
+      </c>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
@@ -3384,11 +3408,7 @@
           <t>Studio 1</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>CSC423</t>
-        </is>
-      </c>
+      <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
@@ -3425,16 +3445,8 @@
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>MAT225</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>MAT225</t>
-        </is>
-      </c>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr"/>
       <c r="I28" t="inlineStr"/>
@@ -3450,7 +3462,11 @@
       <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr"/>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>MIS221</t>
+        </is>
+      </c>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr"/>

</xml_diff>

<commit_message>
Managed to get it tol work abit
</commit_message>
<xml_diff>
--- a/Version 3.0/sheets/final_timetable.xlsx
+++ b/Version 3.0/sheets/final_timetable.xlsx
@@ -501,23 +501,23 @@
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>CSC221</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>CSC221</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>CSC441</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>CSC441</t>
-        </is>
-      </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -550,8 +550,16 @@
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>GST121</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>GST121</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -563,8 +571,16 @@
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>MIS421</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>MIS421</t>
+        </is>
+      </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
@@ -585,7 +601,11 @@
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>MAT226</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -596,11 +616,7 @@
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
@@ -668,19 +684,19 @@
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>CIT242</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>CIT242</t>
+        </is>
+      </c>
       <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>MAT229</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>MAT229</t>
-        </is>
-      </c>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
     </row>
@@ -711,14 +727,18 @@
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>CSC425</t>
-        </is>
-      </c>
+      <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>CSC227</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>CSC227</t>
+        </is>
+      </c>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
     </row>
@@ -770,8 +790,16 @@
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>PHY122</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>PHY122</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -782,8 +810,16 @@
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>CSC121</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>CSC121</t>
+        </is>
+      </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
@@ -802,7 +838,11 @@
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>MIS221</t>
+        </is>
+      </c>
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
@@ -853,7 +893,11 @@
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>CSC223</t>
+        </is>
+      </c>
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
@@ -906,16 +950,8 @@
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>CSC446</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>CSC446</t>
-        </is>
-      </c>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -931,16 +967,8 @@
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>GST221</t>
-        </is>
-      </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>GST221</t>
-        </is>
-      </c>
+      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -967,18 +995,22 @@
       </c>
       <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>MAT225</t>
-        </is>
-      </c>
+      <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr"/>
       <c r="I27" t="inlineStr"/>
-      <c r="J27" t="inlineStr"/>
-      <c r="K27" t="inlineStr"/>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>CIS421</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>CIS421</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1010,8 +1042,16 @@
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr"/>
-      <c r="I29" t="inlineStr"/>
-      <c r="J29" t="inlineStr"/>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>CSC442</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>CSC442</t>
+        </is>
+      </c>
       <c r="K29" t="inlineStr"/>
     </row>
   </sheetData>
@@ -1099,7 +1139,11 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>EDS121</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
@@ -1113,16 +1157,8 @@
           <t>Bio Chem Lab 2</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>CIT121</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>CIT121</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
@@ -1146,8 +1182,16 @@
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>MAT121</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>MAT121</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1157,8 +1201,16 @@
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>MAT225</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>MAT225</t>
+        </is>
+      </c>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
@@ -1178,8 +1230,16 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>CSC446</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>CSC446</t>
+        </is>
+      </c>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
     </row>
@@ -1189,13 +1249,29 @@
           <t>Chem Prac. Lab</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>CSC444</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>CSC444</t>
+        </is>
+      </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>DLD121</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>DLD121</t>
+        </is>
+      </c>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
@@ -1214,8 +1290,16 @@
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>CSC225</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>CSC225</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1230,8 +1314,16 @@
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>BUS124</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>BUS124</t>
+        </is>
+      </c>
       <c r="K9" t="inlineStr"/>
     </row>
     <row r="10">
@@ -1261,8 +1353,16 @@
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>MIS425</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>MIS425</t>
+        </is>
+      </c>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
@@ -1296,8 +1396,16 @@
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>MAT229</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>MAT229</t>
+        </is>
+      </c>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
@@ -1315,17 +1423,17 @@
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>GST122</t>
-        </is>
-      </c>
+      <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr">
         <is>
-          <t>GST122</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr"/>
+          <t>PHY121</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>PHY121</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1341,16 +1449,8 @@
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>CIT224</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>CIT224</t>
-        </is>
-      </c>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1402,14 +1502,10 @@
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr">
         <is>
-          <t>GST121</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>GST121</t>
-        </is>
-      </c>
+          <t>CBS121</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1418,8 +1514,16 @@
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>MIS426</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>MIS426</t>
+        </is>
+      </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
@@ -1436,16 +1540,28 @@
       </c>
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>CSC226</t>
+        </is>
+      </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>TMC121</t>
+          <t>CSC226</t>
         </is>
       </c>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
     </row>
@@ -1464,7 +1580,7 @@
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr">
         <is>
-          <t>CSC223</t>
+          <t>CSC423</t>
         </is>
       </c>
       <c r="J21" t="inlineStr"/>
@@ -1512,16 +1628,8 @@
       </c>
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>CSC121</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>CSC121</t>
-        </is>
-      </c>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
@@ -1538,16 +1646,8 @@
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>CSC224</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>CSC224</t>
-        </is>
-      </c>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr"/>
@@ -1566,17 +1666,17 @@
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>CSC226</t>
-        </is>
-      </c>
+      <c r="H26" t="inlineStr"/>
       <c r="I26" t="inlineStr">
         <is>
-          <t>CSC226</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr"/>
+          <t>CSC224</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>CSC224</t>
+        </is>
+      </c>
       <c r="K26" t="inlineStr"/>
     </row>
     <row r="27">
@@ -1623,16 +1723,20 @@
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>PHY129</t>
-        </is>
-      </c>
+      <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr"/>
-      <c r="J29" t="inlineStr"/>
-      <c r="K29" t="inlineStr"/>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>MIS423</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>MIS423</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1721,8 +1825,16 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>CIT141</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>CIT141</t>
+        </is>
+      </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
@@ -1733,11 +1845,7 @@
           <t>Bio Chem Lab 2</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>CSC221</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
@@ -1756,7 +1864,11 @@
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>TMC121</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
@@ -1789,8 +1901,16 @@
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>CSC223</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>CSC223</t>
+        </is>
+      </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
@@ -1812,17 +1932,17 @@
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>DLD221</t>
+        </is>
+      </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>CSC227</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>CSC227</t>
-        </is>
-      </c>
+          <t>DLD221</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1834,16 +1954,8 @@
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>CST121</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>CST121</t>
-        </is>
-      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
@@ -1895,11 +2007,7 @@
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>MAT121</t>
-        </is>
-      </c>
+      <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
@@ -1930,7 +2038,7 @@
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr">
         <is>
-          <t>CSC225</t>
+          <t>EDS421</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
@@ -1952,10 +2060,22 @@
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>CSC425</t>
+        </is>
+      </c>
       <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>CSC441</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>CSC441</t>
+        </is>
+      </c>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
     </row>
@@ -1966,11 +2086,7 @@
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>CSC423</t>
-        </is>
-      </c>
+      <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
@@ -2026,16 +2142,8 @@
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>CIT221</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>CIT221</t>
-        </is>
-      </c>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
     </row>
@@ -2080,11 +2188,7 @@
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>MAT226</t>
-        </is>
-      </c>
+      <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
@@ -2118,14 +2222,10 @@
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>MAT122</t>
-        </is>
-      </c>
+      <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr">
         <is>
-          <t>MAT122</t>
+          <t>PHY129</t>
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
@@ -2166,16 +2266,8 @@
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>CSC223</t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>CSC223</t>
-        </is>
-      </c>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
     </row>
     <row r="26">
@@ -2190,22 +2282,10 @@
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>EDS121</t>
-        </is>
-      </c>
+      <c r="H26" t="inlineStr"/>
       <c r="I26" t="inlineStr"/>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>DLD221</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>DLD221</t>
-        </is>
-      </c>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2230,8 +2310,16 @@
           <t>Studio 3</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr"/>
-      <c r="C28" t="inlineStr"/>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>BUS326</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>BUS326</t>
+        </is>
+      </c>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
@@ -2251,16 +2339,8 @@
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>CIS421</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>CIS421</t>
-        </is>
-      </c>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr"/>
@@ -2357,12 +2437,12 @@
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>CSC424</t>
+          <t>CIT221</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>CSC424</t>
+          <t>CIT221</t>
         </is>
       </c>
       <c r="K2" t="inlineStr"/>
@@ -2398,8 +2478,16 @@
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>CSC125</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>CSC125</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -2426,16 +2514,8 @@
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>CIT141</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>CIT141</t>
-        </is>
-      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
@@ -2454,11 +2534,7 @@
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>EDS421</t>
-        </is>
-      </c>
+      <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
@@ -2476,11 +2552,7 @@
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>PHY121</t>
-        </is>
-      </c>
+      <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
@@ -2532,7 +2604,11 @@
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>MIS421</t>
+        </is>
+      </c>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
     </row>
@@ -2563,8 +2639,16 @@
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>CSC423</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>CSC423</t>
+        </is>
+      </c>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
@@ -2595,15 +2679,19 @@
       </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>ACC121</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>ACC121</t>
+        </is>
+      </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>TMC421</t>
-        </is>
-      </c>
+      <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
@@ -2636,8 +2724,16 @@
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>CIT121</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>CIT121</t>
+        </is>
+      </c>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
@@ -2654,7 +2750,11 @@
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>MIS423</t>
+        </is>
+      </c>
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
@@ -2670,16 +2770,8 @@
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>CSC221</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>CSC221</t>
-        </is>
-      </c>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr"/>
@@ -2691,17 +2783,17 @@
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>DLD121</t>
-        </is>
-      </c>
+      <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr">
         <is>
-          <t>DLD121</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr"/>
+          <t>MAT122</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>MAT122</t>
+        </is>
+      </c>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
@@ -2719,10 +2811,22 @@
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>CSC425</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>CSC425</t>
+        </is>
+      </c>
       <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>EDS221</t>
+        </is>
+      </c>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
     </row>
@@ -2753,8 +2857,16 @@
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>BUS221</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>BUS221</t>
+        </is>
+      </c>
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr"/>
@@ -2772,16 +2884,8 @@
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>CSC125</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>CSC125</t>
-        </is>
-      </c>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr"/>
     </row>
@@ -2832,16 +2936,8 @@
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr"/>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>CSC425</t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>CSC425</t>
-        </is>
-      </c>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
     </row>
     <row r="28">
@@ -2963,7 +3059,11 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>CSC225</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
@@ -2978,8 +3078,16 @@
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>MAT226</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>MAT226</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
@@ -3067,7 +3175,11 @@
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>MAT225</t>
+        </is>
+      </c>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
@@ -3133,17 +3245,13 @@
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>MAT226</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>MAT226</t>
-        </is>
-      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>BUS326</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
@@ -3158,8 +3266,16 @@
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>CIT224</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>CIT224</t>
+        </is>
+      </c>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
@@ -3193,16 +3309,8 @@
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>PHY122</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>PHY122</t>
-        </is>
-      </c>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
@@ -3248,16 +3356,8 @@
           <t>Hall 307</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>CSC444</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>CSC444</t>
-        </is>
-      </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
@@ -3296,12 +3396,12 @@
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>MAT225</t>
+          <t>GST222</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>MAT225</t>
+          <t>GST222</t>
         </is>
       </c>
       <c r="H20" t="inlineStr"/>
@@ -3316,7 +3416,11 @@
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>MAT121</t>
+        </is>
+      </c>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
@@ -3370,16 +3474,8 @@
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>MAT121</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>MAT121</t>
-        </is>
-      </c>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
@@ -3442,7 +3538,11 @@
           <t>Studio 3</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr"/>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>CBS221</t>
+        </is>
+      </c>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr"/>
@@ -3462,11 +3562,7 @@
       <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>MIS221</t>
-        </is>
-      </c>
+      <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr"/>

</xml_diff>

<commit_message>
Made tweaks to all these files. integrated SA.
</commit_message>
<xml_diff>
--- a/Version 3.0/sheets/final_timetable.xlsx
+++ b/Version 3.0/sheets/final_timetable.xlsx
@@ -501,16 +501,8 @@
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CSC221</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>CSC221</t>
-        </is>
-      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
@@ -550,16 +542,8 @@
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>GST121</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>GST121</t>
-        </is>
-      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -571,16 +555,8 @@
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>MIS421</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>MIS421</t>
-        </is>
-      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
@@ -601,11 +577,7 @@
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>MAT226</t>
-        </is>
-      </c>
+      <c r="K6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -684,19 +656,19 @@
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>CIT242</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>CIT242</t>
-        </is>
-      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>CSC442</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>CSC442</t>
+        </is>
+      </c>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
     </row>
@@ -731,12 +703,12 @@
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr">
         <is>
-          <t>CSC227</t>
+          <t>CSC424</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>CSC227</t>
+          <t>CSC424</t>
         </is>
       </c>
       <c r="J13" t="inlineStr"/>
@@ -790,16 +762,8 @@
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>PHY122</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>PHY122</t>
-        </is>
-      </c>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -810,16 +774,8 @@
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>CSC121</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>CSC121</t>
-        </is>
-      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
@@ -838,11 +794,7 @@
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>MIS221</t>
-        </is>
-      </c>
+      <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
@@ -878,8 +830,16 @@
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr"/>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>DLD221</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>DLD221</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -893,11 +853,7 @@
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>CSC223</t>
-        </is>
-      </c>
+      <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
@@ -1001,16 +957,8 @@
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr"/>
       <c r="I27" t="inlineStr"/>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>CIS421</t>
-        </is>
-      </c>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>CIS421</t>
-        </is>
-      </c>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1042,16 +990,8 @@
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr"/>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>CSC442</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>CSC442</t>
-        </is>
-      </c>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr"/>
     </row>
   </sheetData>
@@ -1139,11 +1079,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>EDS121</t>
-        </is>
-      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
@@ -1175,23 +1111,23 @@
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>CSC425</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>CSC425</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>MAT121</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>MAT121</t>
-        </is>
-      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1201,16 +1137,8 @@
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>MAT225</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>MAT225</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
@@ -1230,16 +1158,8 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>CSC446</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>CSC446</t>
-        </is>
-      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
     </row>
@@ -1249,29 +1169,13 @@
           <t>Chem Prac. Lab</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>CSC444</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>CSC444</t>
-        </is>
-      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>DLD121</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>DLD121</t>
-        </is>
-      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
@@ -1290,16 +1194,8 @@
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>CSC225</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>CSC225</t>
-        </is>
-      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1309,21 +1205,21 @@
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>CSC441</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>CSC441</t>
+        </is>
+      </c>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>BUS124</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>BUS124</t>
-        </is>
-      </c>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
     </row>
     <row r="10">
@@ -1337,8 +1233,16 @@
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>BIO111</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>BIO111</t>
+        </is>
+      </c>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
@@ -1353,16 +1257,8 @@
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>MIS425</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>MIS425</t>
-        </is>
-      </c>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
@@ -1396,16 +1292,8 @@
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>MAT229</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>MAT229</t>
-        </is>
-      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
@@ -1424,16 +1312,8 @@
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>PHY121</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>PHY121</t>
-        </is>
-      </c>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1496,15 +1376,15 @@
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>CBS121</t>
-        </is>
-      </c>
+      <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
     </row>
     <row r="19">
@@ -1514,16 +1394,8 @@
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>MIS426</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>MIS426</t>
-        </is>
-      </c>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
@@ -1540,29 +1412,17 @@
       </c>
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>CSC226</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>CSC226</t>
-        </is>
-      </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>CSC424</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>MAT111</t>
+        </is>
+      </c>
       <c r="K20" t="inlineStr"/>
     </row>
     <row r="21">
@@ -1578,11 +1438,7 @@
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>CSC423</t>
-        </is>
-      </c>
+      <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
     </row>
@@ -1631,7 +1487,11 @@
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
@@ -1667,16 +1527,8 @@
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>CSC224</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>CSC224</t>
-        </is>
-      </c>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr"/>
     </row>
     <row r="27">
@@ -1727,16 +1579,8 @@
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr"/>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>MIS423</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>MIS423</t>
-        </is>
-      </c>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1825,16 +1669,8 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>CIT141</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>CIT141</t>
-        </is>
-      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
@@ -1864,11 +1700,7 @@
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>TMC121</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
@@ -1901,16 +1733,8 @@
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>CSC223</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>CSC223</t>
-        </is>
-      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
@@ -1932,16 +1756,8 @@
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>DLD221</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>DLD221</t>
-        </is>
-      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
@@ -1952,7 +1768,11 @@
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>CSC425</t>
+        </is>
+      </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
@@ -2036,11 +1856,7 @@
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>EDS421</t>
-        </is>
-      </c>
+      <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
@@ -2060,23 +1876,15 @@
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>CSC425</t>
-        </is>
-      </c>
+      <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>CSC441</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>CSC441</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>BIO111</t>
+        </is>
+      </c>
       <c r="K14" t="inlineStr"/>
     </row>
     <row r="15">
@@ -2171,10 +1979,26 @@
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>CHM111</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>CHM111</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>GST111</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>GST111</t>
+        </is>
+      </c>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr"/>
@@ -2194,8 +2018,16 @@
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>MAT111</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>MAT111</t>
+        </is>
+      </c>
       <c r="K21" t="inlineStr"/>
     </row>
     <row r="22">
@@ -2223,11 +2055,7 @@
       </c>
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>PHY129</t>
-        </is>
-      </c>
+      <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr"/>
@@ -2310,16 +2138,8 @@
           <t>Studio 3</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>BUS326</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>BUS326</t>
-        </is>
-      </c>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
@@ -2435,16 +2255,8 @@
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>CIT221</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>CIT221</t>
-        </is>
-      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
     </row>
     <row r="3">
@@ -2478,16 +2290,8 @@
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>CSC125</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>CSC125</t>
-        </is>
-      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -2604,11 +2408,7 @@
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>MIS421</t>
-        </is>
-      </c>
+      <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
     </row>
@@ -2639,16 +2439,8 @@
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>CSC423</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>CSC423</t>
-        </is>
-      </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
@@ -2679,16 +2471,8 @@
       </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>ACC121</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>ACC121</t>
-        </is>
-      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
@@ -2724,16 +2508,8 @@
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>CIT121</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>CIT121</t>
-        </is>
-      </c>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
@@ -2750,11 +2526,7 @@
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>MIS423</t>
-        </is>
-      </c>
+      <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
@@ -2786,12 +2558,12 @@
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr">
         <is>
-          <t>MAT122</t>
+          <t>MAT112</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>MAT122</t>
+          <t>MAT112</t>
         </is>
       </c>
       <c r="F20" t="inlineStr"/>
@@ -2811,22 +2583,10 @@
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>CSC425</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>CSC425</t>
-        </is>
-      </c>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>EDS221</t>
-        </is>
-      </c>
+      <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
     </row>
@@ -2857,16 +2617,8 @@
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>BUS221</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>BUS221</t>
-        </is>
-      </c>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr"/>
@@ -2897,7 +2649,11 @@
       </c>
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr"/>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>CSC442</t>
+        </is>
+      </c>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr"/>
@@ -3061,7 +2817,7 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>CSC225</t>
+          <t>CSC111</t>
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
@@ -3078,16 +2834,8 @@
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>MAT226</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>MAT226</t>
-        </is>
-      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
@@ -3171,15 +2919,19 @@
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>CSC424</t>
+        </is>
+      </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>MAT225</t>
-        </is>
-      </c>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
@@ -3245,11 +2997,7 @@
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>BUS326</t>
-        </is>
-      </c>
+      <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
@@ -3266,16 +3014,8 @@
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>CIT224</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>CIT224</t>
-        </is>
-      </c>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
@@ -3360,7 +3100,11 @@
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>CSC423</t>
+        </is>
+      </c>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr"/>
@@ -3390,20 +3134,24 @@
           <t>LT 1</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>CIS421</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>CIS421</t>
+        </is>
+      </c>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>GST222</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>GST222</t>
-        </is>
-      </c>
+          <t>CHM111</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
@@ -3416,11 +3164,7 @@
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>MAT121</t>
-        </is>
-      </c>
+      <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
@@ -3538,11 +3282,7 @@
           <t>Studio 3</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>CBS221</t>
-        </is>
-      </c>
+      <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr"/>

</xml_diff>